<commit_message>
Adds legal/in for India and the DPDP Act 2023
closes #140
</commit_message>
<xml_diff>
--- a/code/vocab_csv/laws-authorities.xlsx
+++ b/code/vocab_csv/laws-authorities.xlsx
@@ -8,7 +8,8 @@
     <sheet state="visible" name="legal-gb" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="legal-us" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="legal-ie" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="archive" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="legal-in" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="archive" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="529">
   <si>
     <t>Term</t>
   </si>
@@ -1138,6 +1139,27 @@
     <t>legal-ie:law-DPA,legal-eu:law-GDPR</t>
   </si>
   <si>
+    <t>law-DPDP</t>
+  </si>
+  <si>
+    <t>Digital Personal Data Protection Act 2023 (DPDP)</t>
+  </si>
+  <si>
+    <t>loc:IN</t>
+  </si>
+  <si>
+    <t>https://www.meity.gov.in/content/digital-personal-data-protection-act-2023</t>
+  </si>
+  <si>
+    <t>DPA-IN</t>
+  </si>
+  <si>
+    <t>Data Protection Board of India</t>
+  </si>
+  <si>
+    <t>legal-in:law-DPDP</t>
+  </si>
+  <si>
     <t>Label_EN</t>
   </si>
   <si>
@@ -1610,7 +1632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1742,6 +1764,12 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
       <color theme="1"/>
@@ -1813,7 +1841,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1945,19 +1973,22 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2026,6 +2057,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -6084,22 +6119,217 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="B3" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>369</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E3" s="45" t="s">
         <v>370</v>
+      </c>
+      <c r="G3" s="22">
+        <v>45149.0</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="K3" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="43"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="10"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="K6" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="37"/>
+      <c r="H7" s="18"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="37"/>
+      <c r="H8" s="18"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="37"/>
+      <c r="H9" s="18"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10">
+      <c r="C10" s="37"/>
+      <c r="H10" s="18"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11">
+      <c r="H11" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A6:X10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$J6="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:X10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$J6="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:X10">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$J6="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:X5 A11:X143">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>$J2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:X5 A11:X143">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$J2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:X5 A11:X143">
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>$J2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E3"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="2" max="2" width="41.63"/>
+    <col customWidth="1" min="6" max="6" width="25.13"/>
+    <col customWidth="1" min="7" max="7" width="57.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>376</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>377</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>8</v>
@@ -6119,7 +6349,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -6134,7 +6364,7 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>111</v>
@@ -6180,7 +6410,7 @@
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>116</v>
@@ -6224,7 +6454,7 @@
     </row>
     <row r="5">
       <c r="A5" s="30" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>120</v>
@@ -6268,7 +6498,7 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>124</v>
@@ -6312,7 +6542,7 @@
     </row>
     <row r="7">
       <c r="A7" s="30" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>128</v>
@@ -6356,7 +6586,7 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>132</v>
@@ -6400,7 +6630,7 @@
     </row>
     <row r="9">
       <c r="A9" s="30" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>136</v>
@@ -6444,7 +6674,7 @@
     </row>
     <row r="10">
       <c r="A10" s="30" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>140</v>
@@ -6488,7 +6718,7 @@
     </row>
     <row r="11">
       <c r="A11" s="30" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>144</v>
@@ -6532,7 +6762,7 @@
     </row>
     <row r="12">
       <c r="A12" s="30" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>148</v>
@@ -6576,7 +6806,7 @@
     </row>
     <row r="13">
       <c r="A13" s="30" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>152</v>
@@ -6620,7 +6850,7 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>156</v>
@@ -6664,7 +6894,7 @@
     </row>
     <row r="15">
       <c r="A15" s="30" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>160</v>
@@ -6708,7 +6938,7 @@
     </row>
     <row r="16">
       <c r="A16" s="30" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>164</v>
@@ -6752,7 +6982,7 @@
     </row>
     <row r="17">
       <c r="A17" s="30" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>168</v>
@@ -6796,7 +7026,7 @@
     </row>
     <row r="18">
       <c r="A18" s="30" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>172</v>
@@ -6840,7 +7070,7 @@
     </row>
     <row r="19">
       <c r="A19" s="30" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>176</v>
@@ -6897,7 +7127,7 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="13"/>
@@ -6956,7 +7186,7 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="13"/>
@@ -6973,7 +7203,7 @@
     </row>
     <row r="24">
       <c r="A24" s="15" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="B24" s="15"/>
       <c r="D24" s="18"/>
@@ -6988,7 +7218,7 @@
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="B25" s="15"/>
       <c r="D25" s="18"/>
@@ -7003,7 +7233,7 @@
     </row>
     <row r="26">
       <c r="A26" s="15" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="B26" s="15"/>
       <c r="D26" s="18"/>
@@ -7018,7 +7248,7 @@
     </row>
     <row r="27">
       <c r="A27" s="15" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B27" s="15"/>
       <c r="D27" s="18"/>
@@ -7044,7 +7274,7 @@
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="B29" s="15"/>
       <c r="D29" s="18"/>
@@ -7057,7 +7287,7 @@
     </row>
     <row r="30">
       <c r="A30" s="15" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>299</v>
@@ -7078,7 +7308,7 @@
         <v>44848.0</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>19</v>
@@ -7089,7 +7319,7 @@
     </row>
     <row r="31">
       <c r="A31" s="15" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>14</v>
@@ -7110,7 +7340,7 @@
         <v>44848.0</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>19</v>
@@ -7121,7 +7351,7 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="13"/>
@@ -7136,7 +7366,7 @@
     </row>
     <row r="34">
       <c r="A34" s="28" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>309</v>
@@ -7180,7 +7410,7 @@
     </row>
     <row r="35">
       <c r="A35" s="30" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>313</v>
@@ -7224,7 +7454,7 @@
     </row>
     <row r="36">
       <c r="A36" s="15" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>315</v>
@@ -7266,7 +7496,7 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>321</v>
@@ -7308,7 +7538,7 @@
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>325</v>
@@ -7350,7 +7580,7 @@
     </row>
     <row r="39">
       <c r="A39" s="15" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>329</v>
@@ -7392,7 +7622,7 @@
     </row>
     <row r="40">
       <c r="A40" s="15" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>333</v>
@@ -7434,7 +7664,7 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="B43" s="32"/>
       <c r="C43" s="41"/>
@@ -7463,23 +7693,23 @@
     </row>
     <row r="44">
       <c r="A44" s="32" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E44" s="32" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="F44" s="33" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="H44" s="35">
         <v>44650.0</v>
@@ -7510,23 +7740,23 @@
     </row>
     <row r="45">
       <c r="A45" s="32" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="F45" s="33" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="H45" s="35">
         <v>44650.0</v>
@@ -7557,23 +7787,23 @@
     </row>
     <row r="46">
       <c r="A46" s="32" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="C46" s="41"/>
       <c r="D46" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="F46" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="H46" s="35">
         <v>44650.0</v>
@@ -7604,23 +7834,23 @@
     </row>
     <row r="47">
       <c r="A47" s="32" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="H47" s="35">
         <v>44650.0</v>
@@ -7651,23 +7881,23 @@
     </row>
     <row r="48">
       <c r="A48" s="33" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="C48" s="41"/>
       <c r="D48" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="F48" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G48" s="47" t="s">
-        <v>428</v>
+      <c r="G48" s="48" t="s">
+        <v>435</v>
       </c>
       <c r="H48" s="35">
         <v>45093.0</v>
@@ -7696,23 +7926,23 @@
     </row>
     <row r="49">
       <c r="A49" s="32" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>430</v>
-      </c>
-      <c r="C49" s="48"/>
+        <v>437</v>
+      </c>
+      <c r="C49" s="49"/>
       <c r="D49" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="F49" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="H49" s="35">
         <v>44650.0</v>
@@ -7743,23 +7973,23 @@
     </row>
     <row r="50">
       <c r="A50" s="32" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>434</v>
-      </c>
-      <c r="C50" s="48"/>
+        <v>441</v>
+      </c>
+      <c r="C50" s="49"/>
       <c r="D50" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="F50" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="H50" s="35">
         <v>44650.0</v>
@@ -7790,23 +8020,23 @@
     </row>
     <row r="51">
       <c r="A51" s="32" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>438</v>
-      </c>
-      <c r="C51" s="48"/>
+        <v>445</v>
+      </c>
+      <c r="C51" s="49"/>
       <c r="D51" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="F51" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="H51" s="35">
         <v>44650.0</v>
@@ -7837,23 +8067,23 @@
     </row>
     <row r="52">
       <c r="A52" s="32" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>442</v>
-      </c>
-      <c r="C52" s="48"/>
+        <v>449</v>
+      </c>
+      <c r="C52" s="49"/>
       <c r="D52" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="F52" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="H52" s="35">
         <v>44650.0</v>
@@ -7884,23 +8114,23 @@
     </row>
     <row r="53">
       <c r="A53" s="32" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="C53" s="48"/>
+        <v>453</v>
+      </c>
+      <c r="C53" s="49"/>
       <c r="D53" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="F53" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="H53" s="35">
         <v>44650.0</v>
@@ -7931,23 +8161,23 @@
     </row>
     <row r="54">
       <c r="A54" s="32" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>450</v>
-      </c>
-      <c r="C54" s="48"/>
+        <v>457</v>
+      </c>
+      <c r="C54" s="49"/>
       <c r="D54" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="F54" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="H54" s="35">
         <v>44650.0</v>
@@ -7978,23 +8208,23 @@
     </row>
     <row r="55">
       <c r="A55" s="32" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="C55" s="48"/>
+        <v>461</v>
+      </c>
+      <c r="C55" s="49"/>
       <c r="D55" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="F55" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="H55" s="35">
         <v>44650.0</v>
@@ -8025,23 +8255,23 @@
     </row>
     <row r="56">
       <c r="A56" s="32" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="C56" s="48"/>
+        <v>465</v>
+      </c>
+      <c r="C56" s="49"/>
       <c r="D56" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="F56" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G56" s="34" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="H56" s="35">
         <v>44650.0</v>
@@ -8077,9 +8307,9 @@
       <c r="B57" s="32" t="s">
         <v>364</v>
       </c>
-      <c r="C57" s="48"/>
+      <c r="C57" s="49"/>
       <c r="D57" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E57" s="32" t="s">
         <v>361</v>
@@ -8088,7 +8318,7 @@
         <v>42</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H57" s="35">
         <v>44650.0</v>
@@ -8119,23 +8349,23 @@
     </row>
     <row r="58">
       <c r="A58" s="33" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>463</v>
-      </c>
-      <c r="C58" s="48"/>
+        <v>470</v>
+      </c>
+      <c r="C58" s="49"/>
       <c r="D58" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="F58" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G58" s="49" t="s">
-        <v>465</v>
+      <c r="G58" s="50" t="s">
+        <v>472</v>
       </c>
       <c r="H58" s="35">
         <v>45093.0</v>
@@ -8162,23 +8392,23 @@
     </row>
     <row r="59">
       <c r="A59" s="32" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="C59" s="48"/>
+        <v>474</v>
+      </c>
+      <c r="C59" s="49"/>
       <c r="D59" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="F59" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="H59" s="35">
         <v>44650.0</v>
@@ -8209,23 +8439,23 @@
     </row>
     <row r="60">
       <c r="A60" s="33" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>471</v>
-      </c>
-      <c r="C60" s="48"/>
+        <v>478</v>
+      </c>
+      <c r="C60" s="49"/>
       <c r="D60" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="F60" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G60" s="47" t="s">
-        <v>473</v>
+      <c r="G60" s="48" t="s">
+        <v>480</v>
       </c>
       <c r="H60" s="35">
         <v>45093.0</v>
@@ -8252,23 +8482,23 @@
     </row>
     <row r="61">
       <c r="A61" s="32" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>475</v>
-      </c>
-      <c r="C61" s="48"/>
+        <v>482</v>
+      </c>
+      <c r="C61" s="49"/>
       <c r="D61" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E61" s="32" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="F61" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="H61" s="35">
         <v>44650.0</v>
@@ -8299,23 +8529,23 @@
     </row>
     <row r="62">
       <c r="A62" s="32" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="C62" s="48"/>
+        <v>486</v>
+      </c>
+      <c r="C62" s="49"/>
       <c r="D62" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="F62" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="H62" s="35">
         <v>44650.0</v>
@@ -8346,23 +8576,23 @@
     </row>
     <row r="63">
       <c r="A63" s="32" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>483</v>
-      </c>
-      <c r="C63" s="48"/>
+        <v>490</v>
+      </c>
+      <c r="C63" s="49"/>
       <c r="D63" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="F63" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="H63" s="35">
         <v>44650.0</v>
@@ -8393,23 +8623,23 @@
     </row>
     <row r="64">
       <c r="A64" s="32" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>487</v>
-      </c>
-      <c r="C64" s="48"/>
+        <v>494</v>
+      </c>
+      <c r="C64" s="49"/>
       <c r="D64" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E64" s="32" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="F64" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="H64" s="35">
         <v>44650.0</v>
@@ -8440,23 +8670,23 @@
     </row>
     <row r="65">
       <c r="A65" s="32" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>491</v>
-      </c>
-      <c r="C65" s="48"/>
+        <v>498</v>
+      </c>
+      <c r="C65" s="49"/>
       <c r="D65" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E65" s="32" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="F65" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="H65" s="35">
         <v>44650.0</v>
@@ -8487,23 +8717,23 @@
     </row>
     <row r="66">
       <c r="A66" s="33" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>495</v>
-      </c>
-      <c r="C66" s="48"/>
+        <v>502</v>
+      </c>
+      <c r="C66" s="49"/>
       <c r="D66" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="F66" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G66" s="47" t="s">
-        <v>497</v>
+      <c r="G66" s="48" t="s">
+        <v>504</v>
       </c>
       <c r="H66" s="35">
         <v>45093.0</v>
@@ -8530,23 +8760,23 @@
     </row>
     <row r="67">
       <c r="A67" s="32" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>499</v>
-      </c>
-      <c r="C67" s="48"/>
+        <v>506</v>
+      </c>
+      <c r="C67" s="49"/>
       <c r="D67" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F67" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="H67" s="35">
         <v>44650.0</v>
@@ -8577,23 +8807,23 @@
     </row>
     <row r="68">
       <c r="A68" s="32" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>503</v>
-      </c>
-      <c r="C68" s="48"/>
+        <v>510</v>
+      </c>
+      <c r="C68" s="49"/>
       <c r="D68" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E68" s="32" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F68" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="H68" s="35">
         <v>44650.0</v>
@@ -8624,23 +8854,23 @@
     </row>
     <row r="69">
       <c r="A69" s="32" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>507</v>
-      </c>
-      <c r="C69" s="48"/>
+        <v>514</v>
+      </c>
+      <c r="C69" s="49"/>
       <c r="D69" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E69" s="32" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="F69" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="H69" s="35">
         <v>44650.0</v>
@@ -8671,23 +8901,23 @@
     </row>
     <row r="70">
       <c r="A70" s="32" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>511</v>
-      </c>
-      <c r="C70" s="48"/>
+        <v>518</v>
+      </c>
+      <c r="C70" s="49"/>
       <c r="D70" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="F70" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="H70" s="35">
         <v>44650.0</v>
@@ -8718,23 +8948,23 @@
     </row>
     <row r="71">
       <c r="A71" s="32" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>515</v>
-      </c>
-      <c r="C71" s="48"/>
+        <v>522</v>
+      </c>
+      <c r="C71" s="49"/>
       <c r="D71" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E71" s="32" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="F71" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="H71" s="35">
         <v>44650.0</v>
@@ -8765,23 +8995,23 @@
     </row>
     <row r="72">
       <c r="A72" s="32" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>519</v>
-      </c>
-      <c r="C72" s="48"/>
+        <v>526</v>
+      </c>
+      <c r="C72" s="49"/>
       <c r="D72" s="33" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E72" s="32" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="F72" s="32" t="s">
         <v>42</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="H72" s="35">
         <v>44650.0</v>

</xml_diff>

<commit_message>
Fix link in legal-kr and duplicate label in TECH
- legal-kr links had brackets and commas which caused mistakes in the
  parser which interpreted them as multiple links; fixed this by
  removing the bracket data - the law url resolves the same way
- TECH had `tech:InputOutput` defined in two different sheets, which
  caused duplicates in labels; fixed that by keeping the term in core
  only and removing the other term
</commit_message>
<xml_diff>
--- a/code/vocab_csv/laws-authorities.xlsx
+++ b/code/vocab_csv/laws-authorities.xlsx
@@ -1949,7 +1949,7 @@
     <t>loc:KR</t>
   </si>
   <si>
-    <t>https://www.law.go.kr/영문법령/개인정보 보호법/(19234,20230314)</t>
+    <t>https://www.law.go.kr/영문법령/개인정보 보호법/</t>
   </si>
   <si>
     <t>Arthit Suriyawongkul, Jompon Pitaksantayothin</t>
@@ -1961,7 +1961,7 @@
     <t>Credit Information Use and Protection Act (CIA)</t>
   </si>
   <si>
-    <t>https://www.law.go.kr/영문법령/신용정보의 이용 및 보호에 관한 법률/(19234,20230314)</t>
+    <t>https://www.law.go.kr/영문법령/신용정보의 이용 및 보호에 관한 법률/</t>
   </si>
   <si>
     <t>law-LIA</t>
@@ -1970,7 +1970,7 @@
     <t>Act on the Protection and Use of Location Information (LIA)</t>
   </si>
   <si>
-    <t>https://www.law.go.kr/영문법령/위치정보의 보호 및 이용 등에 관한 법률/(18517,20211019)</t>
+    <t>https://www.law.go.kr/영문법령/위치정보의 보호 및 이용 등에 관한 법률/</t>
   </si>
   <si>
     <t>DPA-KR</t>

</xml_diff>